<commit_message>
adição de requisito funcionais ao ICs
</commit_message>
<xml_diff>
--- a/planilha/planilha de ICs - Next Page.xlsx
+++ b/planilha/planilha de ICs - Next Page.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
   <si>
     <t xml:space="preserve">ID_RTM</t>
   </si>
@@ -67,7 +67,8 @@
     <t xml:space="preserve">Concluído</t>
   </si>
   <si>
-    <t xml:space="preserve">github</t>
+    <t xml:space="preserve">https://github.com/victor-angeli/Next-page
+</t>
   </si>
   <si>
     <t xml:space="preserve">Raiz do Projeto </t>
@@ -154,25 +155,143 @@
     <t xml:space="preserve">documentação de regras</t>
   </si>
   <si>
-    <t xml:space="preserve">RF-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir o cadastro de leitores, bibliotecas e livrarias</t>
+    <t xml:space="preserve">RF-01-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve permitir que leitores criem uma conta com nome, e-mail e senha.
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Requisito Funcional </t>
   </si>
   <si>
-    <t xml:space="preserve">RF-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir o login de usuários por e-mail e senha.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir a recuperação de senha via e-mail.</t>
+    <t xml:space="preserve">RF-02-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias criem contas com informações da empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-03-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários façam login usando e-mail, senha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-04-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve validar as credenciais antes de permitir o acesso.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-05-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias cadastrem livros com título, autor, categoria e disponibilidade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-06-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir a atualização de informações dos livros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-07-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir a exclusão de livros do catálogo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-08-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários pesquisem livros por título, autor ou categoria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-09-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve exibir apenas livros disponíveis para aluguel ou compra.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-10-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve permitir que leitores solicitem a compra de livros.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-11-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que leitores solicitem o aluguel de livros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-12-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve registrar a transação de compra ou aluguel.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-13-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve apresentar funcionalidades diferentes para leitores e para bibliotecas/livrarias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-14-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários visualizem seus dados e histórico de transações.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-15-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve atualizar automaticamente o status dos livros após uma compra ou aluguel.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -215,13 +334,13 @@
     </font>
     <font>
       <sz val="15"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="15"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -234,7 +353,27 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -248,7 +387,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +398,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
         <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -309,7 +454,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,75 +475,63 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,7 +562,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -481,21 +614,21 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="50.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="66.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="63.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,227 +660,235 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="52.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="71.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
@@ -760,17 +901,21 @@
       <c r="D10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
@@ -783,122 +928,380 @@
       <c r="D11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="41.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="B12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="D16" s="22"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="20"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="20"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="20"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="14"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="20"/>
+      <c r="C28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="20"/>
+      <c r="C29" s="18"/>
     </row>
     <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="20"/>
+      <c r="C30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="20"/>
+      <c r="C31" s="18"/>
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="20"/>
+      <c r="C32" s="18"/>
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="20"/>
+      <c r="C33" s="18"/>
     </row>
     <row r="34" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="20"/>
+      <c r="C34" s="18"/>
     </row>
     <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="20"/>
+      <c r="C35" s="18"/>
     </row>
     <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="20"/>
+      <c r="C36" s="18"/>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="20"/>
+      <c r="C37" s="18"/>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="21"/>
+      <c r="C38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
conclusão da tabela de iCs atual
</commit_message>
<xml_diff>
--- a/planilha/planilha de ICs - Next Page.xlsx
+++ b/planilha/planilha de ICs - Next Page.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="135">
   <si>
     <t xml:space="preserve">ID_RTM</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">V.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Rosenildo </t>
+    <t xml:space="preserve"> PO</t>
   </si>
   <si>
     <t xml:space="preserve">Concluído</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">V.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Diogo</t>
+    <t xml:space="preserve">Analista</t>
   </si>
   <si>
     <t xml:space="preserve">Requisitos do Sistema, que estão em ID-005,ID-006</t>
@@ -155,7 +155,86 @@
     <t xml:space="preserve">documentação de regras</t>
   </si>
   <si>
+    <t xml:space="preserve">Documentação da regras de negócios</t>
+  </si>
+  <si>
     <t xml:space="preserve">RF-01-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que leitores criem uma conta com nome, e-mail e senha.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisito Funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">detalhamento de requisitos Funcionais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-02-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias criem contas com informações da empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-03-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários façam login usando e-mail, senha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-04-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve validar as credenciais antes de permitir o acesso.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-05-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias cadastrem livros com título, autor, categoria e disponibilidade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-06-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir a atualização de informações dos livros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-07-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir a exclusão de livros do catálogo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-08-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários pesquisem livros por título, autor ou categoria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-09-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve exibir apenas livros disponíveis para aluguel ou compra.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-10-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que leitores solicitem a compra de livros.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-11-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que leitores solicitem o aluguel de livros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-12-DOC</t>
   </si>
   <si>
     <r>
@@ -166,132 +245,519 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">O sistema deve permitir que leitores criem uma conta com nome, e-mail e senha.
+      <t xml:space="preserve">O sistema deve registrar a transação de compra ou aluguel.
 </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Requisito Funcional </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-02-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias criem contas com informações da empresa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-03-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que usuários façam login usando e-mail, senha.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-04-DOC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
+    <t xml:space="preserve">RF-13-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve apresentar funcionalidades diferentes para leitores e para bibliotecas/livrarias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-14-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve permitir que usuários visualizem seus dados e histórico de transações.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-15-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve atualizar automaticamente o status dos livros após uma compra ou aluguel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF-01-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve carregar as páginas principais em até 3 segundos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisito não funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">detalhamento de requisitos não funcionais </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve suportar, no mínimo, 20 usuários simultâneos sem perda de desempenho.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">As senhas dos usuários devem ser armazenadas de forma criptografada.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve exigir autenticação para acesso às áreas restritas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Apenas bibliotecas e livrarias autenticadas podem cadastrar ou editar livros</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A interface deve ser simples e intuitiva, acessível por usuários sem conhecimento técnico.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve funcionar corretamente em navegadores modernos (Chrome, Edge, Firefox).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve manter os dados dos usuários e livros consistentes, mesmo em caso de falha</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve ter backup periódico do banco de dados</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RNF-10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">-DOC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O código deve seguir boas práticas de programação para facilitar manutenção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF-11-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve utilizar controle de versão (GitHub) para rastrear alterações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF-12-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve poder ser implantado em qualquer servidor compatível com Java e Spring Boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF-13-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve funcionar em dispositivos desktop e mobile (via navegador)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN-01-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Um livro pode ser adquirido em formato de compra ou aluguel, mas não ambos no mesmo pedido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Regras de Negócios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detalhamento de Regras de negócios para o next page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN-02-DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O prazo de aluguel deve ser definido pela biblioteca/livraria e exibido ao usuário antes da confirmação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN-03-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O usuário deve estar autenticado para efetuar compras ou aluguéis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">O sistema deve validar as credenciais antes de permitir o acesso.
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-05-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que bibliotecas e livrarias cadastrem livros com título, autor, categoria e disponibilidade.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-06-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir a atualização de informações dos livros.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-07-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir a exclusão de livros do catálogo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-08-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que usuários pesquisem livros por título, autor ou categoria.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-09-DOC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RN-04-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Livros com exemplares esgotados não poderão ser alugados ou comprados até reposição</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">O sistema deve exibir apenas livros disponíveis para aluguel ou compra.
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-10-DOC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RN-05-DOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bibliotecas e livrarias podem cadastrar apenas livros de seu próprio acervo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">O sistema deve permitir que leitores solicitem a compra de livros.
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-11-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que leitores solicitem o aluguel de livros.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-12-DOC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">O sistema deve registrar a transação de compra ou aluguel.
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-13-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve apresentar funcionalidades diferentes para leitores e para bibliotecas/livrarias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-14-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve permitir que usuários visualizem seus dados e histórico de transações.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF-15-DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve atualizar automaticamente o status dos livros após uma compra ou aluguel.</t>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UC-01-MDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro de usuário (UC01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de caso de uso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caso de uso demonstrando a relação de parceiros e usuários</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC-02-MDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login (UC02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC-03-MDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro de Livros (UC03)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UC-04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-MDL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualização e exclusão de livros(UC04)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UC-05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-MDL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Busca de Livros (UC05)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UC-06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-MDL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de Livros (UC06)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UC-07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-MDL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluguel de Livros (UC07)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UC-08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-MDL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualização de perfil e histórico (UC08)</t>
   </si>
 </sst>
 </file>
@@ -346,6 +812,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -355,36 +828,25 @@
     <font>
       <sz val="15"/>
       <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Aptos"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -413,7 +875,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -426,6 +888,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -454,7 +923,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,66 +941,70 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -612,23 +1085,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="66.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="63.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,7 +1195,7 @@
       <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -859,21 +1332,23 @@
       <c r="H8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="71.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="11" t="s">
         <v>46</v>
       </c>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
@@ -886,47 +1361,51 @@
       <c r="H9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -940,20 +1419,22 @@
       <c r="H11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="41.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -967,20 +1448,22 @@
       <c r="H12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -994,20 +1477,22 @@
       <c r="H13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="15"/>
+      <c r="I13" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -1021,20 +1506,22 @@
       <c r="H14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="15"/>
+      <c r="I14" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -1048,20 +1535,22 @@
       <c r="H15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -1075,20 +1564,22 @@
       <c r="H16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -1102,20 +1593,22 @@
       <c r="H17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="52.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1129,20 +1622,22 @@
       <c r="H18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>46</v>
+        <v>67</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -1156,20 +1651,22 @@
       <c r="H19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="49" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>46</v>
+        <v>69</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
@@ -1183,20 +1680,22 @@
       <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>46</v>
+        <v>71</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>20</v>
@@ -1210,20 +1709,22 @@
       <c r="H21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>20</v>
@@ -1237,76 +1738,801 @@
       <c r="H22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I22" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="51.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" customFormat="false" ht="51.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" customFormat="false" ht="52.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J43" s="16"/>
+    </row>
+    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="19" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="19" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="19" t="n">
         <v>46</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="18"/>
-    </row>
-    <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="18"/>
-    </row>
-    <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="18"/>
-    </row>
-    <row r="31" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="18"/>
-    </row>
-    <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="18"/>
-    </row>
-    <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="18"/>
-    </row>
-    <row r="34" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="18"/>
-    </row>
-    <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="18"/>
-    </row>
-    <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="18"/>
-    </row>
-    <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="18"/>
-    </row>
-    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="19"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B47" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="19" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>